<commit_message>
Added another screen for quick interactivity testing
</commit_message>
<xml_diff>
--- a/resources/Cashius.xlsx
+++ b/resources/Cashius.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="125">
   <si>
     <t>Features</t>
   </si>
@@ -361,6 +361,36 @@
   </si>
   <si>
     <t>Concert</t>
+  </si>
+  <si>
+    <t>Screen Transitions (ON/OFF)</t>
+  </si>
+  <si>
+    <t>Articles</t>
+  </si>
+  <si>
+    <t>Flash is Dead, Long Live HTML5!</t>
+  </si>
+  <si>
+    <t>Hybrid Adventures:</t>
+  </si>
+  <si>
+    <t>SPA</t>
+  </si>
+  <si>
+    <t>Native vs. Mobile</t>
+  </si>
+  <si>
+    <t>Hybrid Trend</t>
+  </si>
+  <si>
+    <t>iOS WebView, WebGL defaultly on, …</t>
+  </si>
+  <si>
+    <t>Canvas vs. HTML/CSS layout inconsistencies</t>
+  </si>
+  <si>
+    <t>Canvas vs. HTML/CSS performance</t>
   </si>
 </sst>
 </file>
@@ -714,7 +744,7 @@
   <dimension ref="C3:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -938,6 +968,9 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
       <c r="F13" s="2" t="s">
         <v>28</v>
       </c>
@@ -990,7 +1023,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="6:14">
+    <row r="17" spans="4:14">
       <c r="K17" t="s">
         <v>65</v>
       </c>
@@ -998,7 +1031,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="6:14">
+    <row r="18" spans="4:14">
       <c r="F18" s="2" t="s">
         <v>32</v>
       </c>
@@ -1012,7 +1045,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="6:14">
+    <row r="19" spans="4:14">
       <c r="F19" t="s">
         <v>33</v>
       </c>
@@ -1023,7 +1056,10 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="6:14">
+    <row r="20" spans="4:14">
+      <c r="D20" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="F20" t="s">
         <v>34</v>
       </c>
@@ -1034,7 +1070,10 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="6:14">
+    <row r="21" spans="4:14">
+      <c r="D21" t="s">
+        <v>117</v>
+      </c>
       <c r="K21" t="s">
         <v>68</v>
       </c>
@@ -1045,7 +1084,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="6:14">
+    <row r="22" spans="4:14">
+      <c r="D22" t="s">
+        <v>122</v>
+      </c>
       <c r="F22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1056,7 +1098,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="6:14">
+    <row r="23" spans="4:14">
       <c r="F23" t="s">
         <v>47</v>
       </c>
@@ -1067,7 +1109,10 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="6:14">
+    <row r="24" spans="4:14">
+      <c r="D24" t="s">
+        <v>118</v>
+      </c>
       <c r="K24" t="s">
         <v>72</v>
       </c>
@@ -1075,7 +1120,10 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="6:14">
+    <row r="25" spans="4:14">
+      <c r="D25" t="s">
+        <v>119</v>
+      </c>
       <c r="J25" t="s">
         <v>48</v>
       </c>
@@ -1086,7 +1134,10 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="6:14">
+    <row r="26" spans="4:14">
+      <c r="D26" t="s">
+        <v>120</v>
+      </c>
       <c r="K26" t="s">
         <v>74</v>
       </c>
@@ -1094,7 +1145,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="6:14">
+    <row r="27" spans="4:14">
+      <c r="D27" t="s">
+        <v>121</v>
+      </c>
       <c r="K27" t="s">
         <v>75</v>
       </c>
@@ -1102,27 +1156,33 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="6:14">
+    <row r="28" spans="4:14">
+      <c r="D28" t="s">
+        <v>123</v>
+      </c>
       <c r="K28" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="6:14">
+    <row r="29" spans="4:14">
+      <c r="D29" t="s">
+        <v>124</v>
+      </c>
       <c r="K29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="6:14">
+    <row r="30" spans="4:14">
       <c r="K30" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="6:14">
+    <row r="31" spans="4:14">
       <c r="K31" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="6:14">
+    <row r="32" spans="4:14">
       <c r="K32" t="s">
         <v>80</v>
       </c>

</xml_diff>